<commit_message>
US-14022 [IMP] Fix cell protection + fix background filling in assets rows
</commit_message>
<xml_diff>
--- a/bin/addons/product_asset/report/Asset_Reference_Template.xlsx
+++ b/bin/addons/product_asset/report/Asset_Reference_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="10995"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22125" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Mock-up" sheetId="1" r:id="rId1"/>
@@ -141,7 +141,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -285,6 +285,21 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="35">
@@ -701,7 +716,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -735,19 +750,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -755,6 +757,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1079,7 +1101,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1089,7 +1111,7 @@
     <col min="4" max="4" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="61.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="61.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="25.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="26.5703125" style="1" customWidth="1"/>
     <col min="11" max="11" width="24" style="1" customWidth="1"/>
@@ -1097,41 +1119,41 @@
     <col min="13" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" s="21" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="18" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1150,7 +1172,7 @@
       <c r="F2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="17"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="6" t="s">
         <v>32</v>
       </c>
@@ -1184,7 +1206,7 @@
       <c r="F3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="17"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="6" t="s">
         <v>33</v>
       </c>
@@ -1220,7 +1242,7 @@
       <c r="F4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="17"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="6" t="s">
         <v>34</v>
       </c>
@@ -1256,7 +1278,7 @@
       <c r="F5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="17"/>
+      <c r="G5" s="13"/>
       <c r="H5" s="6" t="s">
         <v>35</v>
       </c>
@@ -1276,7 +1298,7 @@
   </sheetData>
   <autoFilter ref="A1:L5"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1478,14 +1500,14 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="14"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="1" t="s">
         <v>29</v>
       </c>

</xml_diff>